<commit_message>
Adding example how to export only specific worksheets
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/workspaces/tools/excel-worksheet-to-csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EA404B-73FE-C34D-A016-D4B093305151}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757F254D-1DFF-3240-9130-50DC9E5C9FF3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{967F58AF-1BEF-1945-8587-287B71EDB81B}"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{967F58AF-1BEF-1945-8587-287B71EDB81B}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet 1" sheetId="1" r:id="rId1"/>
     <sheet name="Another data set" sheetId="2" r:id="rId2"/>
+    <sheet name="Last" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="43">
   <si>
     <t>data1</t>
   </si>
@@ -151,6 +152,15 @@
   </si>
   <si>
     <t>third</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>great</t>
   </si>
 </sst>
 </file>
@@ -849,7 +859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00347926-0708-0442-B42C-C861981ECEEC}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -1188,4 +1198,349 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB1B8FA-3071-C54F-9D78-6B53020D0B86}">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>60</v>
+      </c>
+      <c r="C7">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>70</v>
+      </c>
+      <c r="C8">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>80</v>
+      </c>
+      <c r="C9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>90</v>
+      </c>
+      <c r="C10">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>110</v>
+      </c>
+      <c r="C12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>120</v>
+      </c>
+      <c r="C13">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>130</v>
+      </c>
+      <c r="C14">
+        <v>-21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>140</v>
+      </c>
+      <c r="C15">
+        <v>-31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>150</v>
+      </c>
+      <c r="C16">
+        <v>-41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>160</v>
+      </c>
+      <c r="C17">
+        <v>-51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>170</v>
+      </c>
+      <c r="C18">
+        <v>-61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>180</v>
+      </c>
+      <c r="C19">
+        <v>-71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>190</v>
+      </c>
+      <c r="C20">
+        <v>-81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>200</v>
+      </c>
+      <c r="C21">
+        <v>-91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>210</v>
+      </c>
+      <c r="C22">
+        <v>-101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>220</v>
+      </c>
+      <c r="C23">
+        <v>-111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>230</v>
+      </c>
+      <c r="C24">
+        <v>-121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>240</v>
+      </c>
+      <c r="C25">
+        <v>-131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>250</v>
+      </c>
+      <c r="C26">
+        <v>-141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>260</v>
+      </c>
+      <c r="C27">
+        <v>-151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>270</v>
+      </c>
+      <c r="C28">
+        <v>-161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>280</v>
+      </c>
+      <c r="C29">
+        <v>-171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>290</v>
+      </c>
+      <c r="C30">
+        <v>-181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>